<commit_message>
update Chromedriver to 2.37
</commit_message>
<xml_diff>
--- a/data/VHSuser.xlsx
+++ b/data/VHSuser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>System Manager</t>
   </si>
   <si>
-    <t>1111</t>
+    <t>111111</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>